<commit_message>
core.py: soft_approach uses 1 less node. CheatSheet & softApproach example updated.
</commit_message>
<xml_diff>
--- a/docs/cheat_sheet/node_calculator_cheat_sheet.xlsx
+++ b/docs/cheat_sheet/node_calculator_cheat_sheet.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{063E1D92-D4EA-45A5-9184-250410DC904A}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58A9FDDF-141A-42BC-9482-6300DE1BFD69}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="103">
   <si>
     <t>Op</t>
   </si>
@@ -1270,6 +1270,39 @@
   </si>
   <si>
     <t>NodeCalculator cheat sheet</t>
+  </si>
+  <si>
+    <t>Convenience Functions</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>transform()</t>
+  </si>
+  <si>
+    <t>locator()</t>
+  </si>
+  <si>
+    <t>create_node()</t>
+  </si>
+  <si>
+    <t>noca.transform("myTransform", parent="myParent")</t>
+  </si>
+  <si>
+    <t>noca.locator("myLocator", attrs="translation")</t>
+  </si>
+  <si>
+    <t>noca.create_node("nurbsCurve", "myCurve")</t>
+  </si>
+  <si>
+    <t>Create any node type (as NcNode instance).</t>
+  </si>
+  <si>
+    <t>Create transform node (as NcNode instance).</t>
+  </si>
+  <si>
+    <t>Create locator node (as NcNode instance).</t>
   </si>
 </sst>
 </file>
@@ -1700,7 +1733,7 @@
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
@@ -1797,6 +1830,10 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="7" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2756,10 +2793,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:G58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2770,15 +2807,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="64" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
+      <c r="B1" s="64"/>
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
     </row>
     <row r="2" spans="1:7" s="41" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15"/>
@@ -2790,15 +2827,15 @@
       <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="63" t="s">
+      <c r="A3" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="65"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
@@ -2815,12 +2852,12 @@
       <c r="C6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="69" t="s">
+      <c r="D6" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="70"/>
-      <c r="F6" s="70"/>
-      <c r="G6" s="71"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
+      <c r="G6" s="73"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
@@ -2828,12 +2865,12 @@
       <c r="C7" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="53" t="s">
+      <c r="D7" s="55" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="54"/>
-      <c r="F7" s="54"/>
-      <c r="G7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="56"/>
+      <c r="G7" s="57"/>
     </row>
     <row r="8" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
@@ -2850,11 +2887,11 @@
       <c r="C9" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="D9" s="65" t="s">
+      <c r="D9" s="67" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="64"/>
-      <c r="F9" s="64"/>
+      <c r="E9" s="66"/>
+      <c r="F9" s="66"/>
       <c r="G9" s="3"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2863,11 +2900,11 @@
       <c r="C10" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="68" t="s">
         <v>14</v>
       </c>
-      <c r="E10" s="67"/>
-      <c r="F10" s="68"/>
+      <c r="E10" s="69"/>
+      <c r="F10" s="70"/>
       <c r="G10" s="3"/>
     </row>
     <row r="11" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2884,10 +2921,10 @@
       <c r="B12" s="3"/>
       <c r="C12" s="5"/>
       <c r="D12" s="5"/>
-      <c r="E12" s="64" t="s">
+      <c r="E12" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="F12" s="64"/>
+      <c r="F12" s="66"/>
       <c r="G12" s="5"/>
     </row>
     <row r="13" spans="1:7" ht="45" customHeight="1" x14ac:dyDescent="0.25">
@@ -2895,10 +2932,10 @@
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
       <c r="D13" s="5"/>
-      <c r="E13" s="56" t="s">
+      <c r="E13" s="58" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="57"/>
+      <c r="F13" s="59"/>
       <c r="G13" s="3"/>
     </row>
     <row r="14" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -2911,10 +2948,10 @@
       <c r="G14" s="3"/>
     </row>
     <row r="15" spans="1:7" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A15" s="60" t="s">
+      <c r="A15" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="B15" s="58" t="s">
+      <c r="B15" s="60" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="44" t="s">
@@ -2934,8 +2971,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="61"/>
-      <c r="B16" s="59"/>
+      <c r="A16" s="63"/>
+      <c r="B16" s="61"/>
       <c r="C16" s="47" t="s">
         <v>1</v>
       </c>
@@ -3068,89 +3105,110 @@
       </c>
     </row>
     <row r="24" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="26" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A26" s="62" t="s">
+    <row r="25" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A25" s="64" t="s">
         <v>56</v>
       </c>
-      <c r="B26" s="62"/>
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-    </row>
-    <row r="27" spans="1:7" s="41" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="15"/>
+      <c r="B25" s="64"/>
+      <c r="C25" s="64"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="64"/>
+      <c r="F25" s="64"/>
+      <c r="G25" s="64"/>
+    </row>
+    <row r="26" spans="1:7" s="41" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="15"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="15"/>
+      <c r="E26" s="15"/>
+      <c r="F26" s="15"/>
+      <c r="G26" s="15"/>
+    </row>
+    <row r="27" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="28" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="27" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="27" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="27" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="1:7" s="27" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" s="78" t="s">
+        <v>45</v>
+      </c>
+      <c r="B31" s="78"/>
+      <c r="C31" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>49</v>
+      </c>
+      <c r="E31" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="F31" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="35" t="s">
+        <v>49</v>
+      </c>
+    </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="76" t="s">
-        <v>45</v>
-      </c>
-      <c r="B32" s="76"/>
+      <c r="A32" s="78" t="s">
+        <v>47</v>
+      </c>
+      <c r="B32" s="78"/>
       <c r="C32" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D32" s="34" t="s">
-        <v>49</v>
+      <c r="D32" s="22" t="s">
+        <v>78</v>
       </c>
       <c r="E32" s="20" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="G32" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="76" t="s">
-        <v>47</v>
-      </c>
-      <c r="B33" s="76"/>
+      <c r="A33" s="78" t="s">
+        <v>44</v>
+      </c>
+      <c r="B33" s="78"/>
       <c r="C33" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="D33" s="22" t="s">
-        <v>78</v>
+      <c r="D33" s="34" t="s">
+        <v>49</v>
       </c>
       <c r="E33" s="20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="F33" s="21" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="G33" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="76" t="s">
-        <v>44</v>
-      </c>
-      <c r="B34" s="76"/>
+      <c r="A34" s="78" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="78"/>
       <c r="C34" s="33" t="s">
         <v>49</v>
       </c>
@@ -3158,20 +3216,20 @@
         <v>49</v>
       </c>
       <c r="E34" s="20" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="F34" s="21" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="G34" s="35" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="76" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="76"/>
+      <c r="A35" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="B35" s="78"/>
       <c r="C35" s="33" t="s">
         <v>49</v>
       </c>
@@ -3179,185 +3237,245 @@
         <v>49</v>
       </c>
       <c r="E35" s="20" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F35" s="21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G35" s="35" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="76" t="s">
-        <v>48</v>
-      </c>
-      <c r="B36" s="76"/>
-      <c r="C36" s="33" t="s">
-        <v>49</v>
-      </c>
-      <c r="D36" s="34" t="s">
-        <v>49</v>
-      </c>
-      <c r="E36" s="20" t="s">
-        <v>80</v>
-      </c>
-      <c r="F36" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="G36" s="35" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="37" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="38" spans="1:7" s="23" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="1:7" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
-      <c r="A41" s="62" t="s">
+    <row r="39" spans="1:7" s="53" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A39" s="64" t="s">
+        <v>92</v>
+      </c>
+      <c r="B39" s="64"/>
+      <c r="C39" s="64"/>
+      <c r="D39" s="64"/>
+      <c r="E39" s="64"/>
+      <c r="F39" s="64"/>
+      <c r="G39" s="64"/>
+    </row>
+    <row r="40" spans="1:7" s="53" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="1:7" s="53" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A41" s="77" t="s">
+        <v>93</v>
+      </c>
+      <c r="B41" s="77"/>
+      <c r="C41" s="40" t="s">
+        <v>59</v>
+      </c>
+      <c r="D41" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="E41" s="40"/>
+      <c r="F41" s="1"/>
+    </row>
+    <row r="42" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="75" t="s">
+        <v>94</v>
+      </c>
+      <c r="B42" s="75"/>
+      <c r="C42" s="19" t="s">
+        <v>101</v>
+      </c>
+      <c r="D42" s="75" t="s">
+        <v>97</v>
+      </c>
+      <c r="E42" s="75"/>
+    </row>
+    <row r="43" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="75" t="s">
+        <v>95</v>
+      </c>
+      <c r="B43" s="75"/>
+      <c r="C43" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="D43" s="75" t="s">
+        <v>98</v>
+      </c>
+      <c r="E43" s="75"/>
+    </row>
+    <row r="44" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="75" t="s">
+        <v>96</v>
+      </c>
+      <c r="B44" s="75"/>
+      <c r="C44" s="19" t="s">
+        <v>100</v>
+      </c>
+      <c r="D44" s="75" t="s">
+        <v>99</v>
+      </c>
+      <c r="E44" s="75"/>
+    </row>
+    <row r="45" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="54"/>
+      <c r="B45" s="54"/>
+      <c r="C45" s="1"/>
+      <c r="D45" s="54"/>
+      <c r="E45" s="54"/>
+    </row>
+    <row r="48" spans="1:7" s="53" customFormat="1" ht="36.75" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A48" s="64" t="s">
         <v>57</v>
       </c>
-      <c r="B41" s="62"/>
-      <c r="C41" s="62"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="62"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="62"/>
-    </row>
-    <row r="42" spans="1:7" s="36" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="43" spans="1:7" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A43" s="75" t="s">
+      <c r="B48" s="64"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="64"/>
+      <c r="E48" s="64"/>
+      <c r="F48" s="64"/>
+      <c r="G48" s="64"/>
+    </row>
+    <row r="49" spans="1:6" s="53" customFormat="1" ht="7.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="1:6" s="36" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A50" s="77" t="s">
         <v>58</v>
       </c>
-      <c r="B43" s="75"/>
-      <c r="C43" s="40" t="s">
+      <c r="B50" s="77"/>
+      <c r="C50" s="40" t="s">
         <v>59</v>
       </c>
-      <c r="D43" s="40" t="s">
+      <c r="D50" s="40" t="s">
         <v>63</v>
       </c>
-      <c r="E43" s="40"/>
-      <c r="F43" s="1"/>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A44" s="73" t="s">
+      <c r="E50" s="40"/>
+      <c r="F50" s="1"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="75" t="s">
         <v>45</v>
       </c>
-      <c r="B44" s="73"/>
-      <c r="C44" s="19" t="s">
+      <c r="B51" s="75"/>
+      <c r="C51" s="19" t="s">
         <v>72</v>
       </c>
-      <c r="D44" s="73" t="s">
+      <c r="D51" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="E44" s="73"/>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A45" s="74" t="s">
+      <c r="E51" s="75"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="76" t="s">
         <v>50</v>
       </c>
-      <c r="B45" s="74"/>
-      <c r="C45" s="24" t="s">
+      <c r="B52" s="76"/>
+      <c r="C52" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="D45" s="74" t="s">
+      <c r="D52" s="76" t="s">
         <v>61</v>
       </c>
-      <c r="E45" s="74"/>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="72" t="s">
+      <c r="E52" s="76"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="74" t="s">
         <v>51</v>
       </c>
-      <c r="B46" s="72"/>
-      <c r="C46" s="18" t="s">
+      <c r="B53" s="74"/>
+      <c r="C53" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D46" s="72" t="s">
+      <c r="D53" s="74" t="s">
         <v>62</v>
       </c>
-      <c r="E46" s="72"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="25"/>
-      <c r="B47" s="25"/>
-      <c r="C47" s="26"/>
-      <c r="D47" s="25"/>
-      <c r="E47" s="25"/>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A48" s="73" t="s">
+      <c r="E53" s="74"/>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="25"/>
+      <c r="B54" s="25"/>
+      <c r="C54" s="26"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="75" t="s">
         <v>64</v>
       </c>
-      <c r="B48" s="73"/>
-      <c r="C48" s="19" t="s">
+      <c r="B55" s="75"/>
+      <c r="C55" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="D48" s="73" t="s">
+      <c r="D55" s="75" t="s">
         <v>68</v>
       </c>
-      <c r="E48" s="73"/>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A49" s="74" t="s">
+      <c r="E55" s="75"/>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="76" t="s">
         <v>65</v>
       </c>
-      <c r="B49" s="74"/>
-      <c r="C49" s="24" t="s">
+      <c r="B56" s="76"/>
+      <c r="C56" s="24" t="s">
         <v>54</v>
       </c>
-      <c r="D49" s="74" t="s">
+      <c r="D56" s="76" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="74"/>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="74" t="s">
+      <c r="E56" s="76"/>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A57" s="76" t="s">
         <v>66</v>
       </c>
-      <c r="B50" s="74"/>
-      <c r="C50" s="24" t="s">
+      <c r="B57" s="76"/>
+      <c r="C57" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="D50" s="74" t="s">
+      <c r="D57" s="76" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="74"/>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="74" t="s">
+      <c r="E57" s="76"/>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A58" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="B51" s="74"/>
-      <c r="C51" s="24" t="s">
+      <c r="B58" s="76"/>
+      <c r="C58" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="D51" s="74" t="s">
+      <c r="D58" s="76" t="s">
         <v>74</v>
       </c>
-      <c r="E51" s="74"/>
+      <c r="E58" s="76"/>
     </row>
   </sheetData>
-  <mergeCells count="32">
-    <mergeCell ref="D50:E50"/>
-    <mergeCell ref="D51:E51"/>
+  <mergeCells count="40">
+    <mergeCell ref="D57:E57"/>
+    <mergeCell ref="D58:E58"/>
+    <mergeCell ref="A31:B31"/>
     <mergeCell ref="A32:B32"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
-    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="A51:B51"/>
+    <mergeCell ref="A52:B52"/>
+    <mergeCell ref="A53:B53"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A57:B57"/>
+    <mergeCell ref="A58:B58"/>
+    <mergeCell ref="D51:E51"/>
+    <mergeCell ref="D52:E52"/>
+    <mergeCell ref="D53:E53"/>
+    <mergeCell ref="D55:E55"/>
+    <mergeCell ref="D56:E56"/>
+    <mergeCell ref="A50:B50"/>
+    <mergeCell ref="A25:G25"/>
+    <mergeCell ref="A48:G48"/>
+    <mergeCell ref="A41:B41"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="D42:E42"/>
+    <mergeCell ref="A39:G39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="D43:E43"/>
     <mergeCell ref="A44:B44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="A48:B48"/>
-    <mergeCell ref="A49:B49"/>
-    <mergeCell ref="A50:B50"/>
-    <mergeCell ref="A51:B51"/>
     <mergeCell ref="D44:E44"/>
-    <mergeCell ref="D45:E45"/>
-    <mergeCell ref="D46:E46"/>
-    <mergeCell ref="D48:E48"/>
-    <mergeCell ref="D49:E49"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="A26:G26"/>
-    <mergeCell ref="A41:G41"/>
     <mergeCell ref="D7:G7"/>
     <mergeCell ref="E13:F13"/>
     <mergeCell ref="B15:B16"/>
@@ -3370,7 +3488,7 @@
     <mergeCell ref="D6:G6"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="53" orientation="landscape" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="49" fitToWidth="0" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>